<commit_message>
DAC freq increase and TXCO correction update
</commit_message>
<xml_diff>
--- a/Scheme/DAC_freq.xlsx
+++ b/Scheme/DAC_freq.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>1 nyquist</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Attenuation, db</t>
+  </si>
+  <si>
+    <t>1n</t>
+  </si>
+  <si>
+    <t>2n</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -480,6 +486,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,14 +785,21 @@
     <col min="24" max="24" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="26">
-        <f>48000*3760/1000000</f>
-        <v>180.48</v>
+        <f>48000*4160/1000000</f>
+        <v>199.68</v>
       </c>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
@@ -794,9 +810,12 @@
       <c r="J2" s="23"/>
       <c r="K2" s="23">
         <f>C2/2</f>
-        <v>90.24</v>
-      </c>
-      <c r="L2" s="23"/>
+        <v>99.84</v>
+      </c>
+      <c r="L2" s="23">
+        <f>K2*2</f>
+        <v>199.68</v>
+      </c>
       <c r="M2" s="23"/>
       <c r="N2" s="23"/>
       <c r="O2" s="23"/>
@@ -836,7 +855,7 @@
       </c>
       <c r="D4" s="10">
         <f>C2*0.4</f>
-        <v>72.191999999999993</v>
+        <v>79.872000000000014</v>
       </c>
       <c r="E4" s="8">
         <f>C4</f>
@@ -844,19 +863,19 @@
       </c>
       <c r="F4" s="3">
         <f>D4</f>
-        <v>72.191999999999993</v>
+        <v>79.872000000000014</v>
       </c>
       <c r="G4" s="8">
         <f>F4</f>
-        <v>72.191999999999993</v>
+        <v>79.872000000000014</v>
       </c>
       <c r="H4" s="3">
         <f>E5</f>
-        <v>108.288</v>
+        <v>119.80799999999999</v>
       </c>
       <c r="I4" s="12">
         <f>(G4+H4)/2</f>
-        <v>90.24</v>
+        <v>99.84</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
@@ -872,31 +891,31 @@
       </c>
       <c r="C5" s="8">
         <f>C2*0.2</f>
-        <v>36.095999999999997</v>
+        <v>39.936000000000007</v>
       </c>
       <c r="D5" s="10">
         <f>C2*0.4</f>
-        <v>72.191999999999993</v>
+        <v>79.872000000000014</v>
       </c>
       <c r="E5" s="8">
         <f>C2-D5</f>
-        <v>108.288</v>
+        <v>119.80799999999999</v>
       </c>
       <c r="F5" s="3">
         <f>C2-C5</f>
-        <v>144.38399999999999</v>
+        <v>159.744</v>
       </c>
       <c r="G5" s="8">
         <f>F5</f>
-        <v>144.38399999999999</v>
+        <v>159.744</v>
       </c>
       <c r="H5" s="3">
         <f>E6</f>
-        <v>216.57599999999999</v>
+        <v>239.61600000000001</v>
       </c>
       <c r="I5" s="12">
         <f t="shared" ref="I5:I6" si="0">(G5+H5)/2</f>
-        <v>180.48</v>
+        <v>199.68</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
@@ -912,31 +931,31 @@
       </c>
       <c r="C6" s="8">
         <f>C2*0.2</f>
-        <v>36.095999999999997</v>
+        <v>39.936000000000007</v>
       </c>
       <c r="D6" s="10">
         <f>C2*0.4</f>
-        <v>72.191999999999993</v>
+        <v>79.872000000000014</v>
       </c>
       <c r="E6" s="8">
         <f>C2+C6</f>
-        <v>216.57599999999999</v>
+        <v>239.61600000000001</v>
       </c>
       <c r="F6" s="3">
         <f>C2+D6</f>
-        <v>252.67199999999997</v>
+        <v>279.55200000000002</v>
       </c>
       <c r="G6" s="8">
         <f>F6</f>
-        <v>252.67199999999997</v>
+        <v>279.55200000000002</v>
       </c>
       <c r="H6" s="3">
         <f>E7</f>
-        <v>288.76799999999997</v>
+        <v>319.488</v>
       </c>
       <c r="I6" s="12">
         <f t="shared" si="0"/>
-        <v>270.71999999999997</v>
+        <v>299.52</v>
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
@@ -955,15 +974,15 @@
       </c>
       <c r="D7" s="11">
         <f>C2*0.4</f>
-        <v>72.191999999999993</v>
+        <v>79.872000000000014</v>
       </c>
       <c r="E7" s="9">
         <f>C2*2-D7</f>
-        <v>288.76799999999997</v>
+        <v>319.488</v>
       </c>
       <c r="F7" s="4">
         <f>C2*2-C7</f>
-        <v>360.96</v>
+        <v>399.36</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="4"/>

</xml_diff>